<commit_message>
Changes to allow for unit testing
</commit_message>
<xml_diff>
--- a/UT.Vol.BLL/HelperFiles/Skill.xlsx
+++ b/UT.Vol.BLL/HelperFiles/Skill.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
   <si>
     <t>Table</t>
   </si>
@@ -43,25 +43,16 @@
     <t>SQL Server 2010</t>
   </si>
   <si>
-    <t>85CD9529-322B-4B63-9F04-9E03924999BE</t>
-  </si>
-  <si>
     <t>C87F23E9-8F8C-406D-9FBF-E15043179F09</t>
   </si>
   <si>
     <t>Redditor</t>
   </si>
   <si>
-    <t>6497B3D4-A86F-441C-9856-5E00EB410B9D</t>
-  </si>
-  <si>
     <t>990B091D-6A0D-4543-B766-C37B684F8081</t>
   </si>
   <si>
     <t>4Chan Troll</t>
-  </si>
-  <si>
-    <t>F8389EDE-E282-4AAE-B6B7-94A99FF1D85A</t>
   </si>
 </sst>
 </file>
@@ -155,9 +146,6 @@
       <c t="s" r="C2">
         <v>9</v>
       </c>
-      <c t="s" r="D2">
-        <v>10</v>
-      </c>
       <c r="E2">
         <v>0</v>
       </c>
@@ -165,8 +153,8 @@
         <v>0</v>
       </c>
       <c t="str" r="G2">
-        <f>((((((((((((((((((((("INSERT INTO " &amp; A2) &amp;" (") &amp; $B$1) &amp; ",") &amp; $C$1) &amp; ",") &amp; $D$1) &amp; ",") &amp; $E$1) &amp; ",") &amp; $F$1) &amp; ") VALUES('") &amp; RC[-5]) &amp;"','") &amp; RC[-4]) &amp;"','") &amp; RC[-3]) &amp;"','") &amp; RC[-2]) &amp;"','") &amp; RC[-1]) &amp; "')"</f>
-        <v>INSERT INTO [Vol].[tblSkill] (SkillID,SkillName,MstrSkillID,ReqCert,ActiveFlg) VALUES('153B9006-1488-4CA1-950A-32E28F7B699D','SQL Server 2010','85CD9529-322B-4B63-9F04-9E03924999BE','0','0')</v>
+        <f>((((((((((((((((("INSERT INTO " &amp; A2) &amp;" (") &amp; $B$1) &amp; ",") &amp; $C$1) &amp; ",") &amp; $E$1) &amp; ",") &amp; $F$1) &amp; ") VALUES('") &amp; RC[-5]) &amp;"','") &amp; RC[-4]) &amp;"','") &amp; RC[-2]) &amp;"','") &amp; RC[-1]) &amp; "')"</f>
+        <v>INSERT INTO [Vol].[tblSkill] (SkillID,SkillName,ReqCert,ActiveFlg) VALUES('153B9006-1488-4CA1-950A-32E28F7B699D','SQL Server 2010','0','0')</v>
       </c>
     </row>
     <row r="3">
@@ -174,13 +162,13 @@
         <v>7</v>
       </c>
       <c t="s" r="B3">
+        <v>10</v>
+      </c>
+      <c t="s" r="C3">
         <v>11</v>
       </c>
-      <c t="s" r="C3">
-        <v>12</v>
-      </c>
       <c t="s" r="D3">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -190,7 +178,7 @@
       </c>
       <c t="str" r="G3">
         <f>((((((((((((((((((((("INSERT INTO " &amp; A3) &amp;" (") &amp; $B$1) &amp; ",") &amp; $C$1) &amp; ",") &amp; $D$1) &amp; ",") &amp; $E$1) &amp; ",") &amp; $F$1) &amp; ") VALUES('") &amp; RC[-5]) &amp;"','") &amp; RC[-4]) &amp;"','") &amp; RC[-3]) &amp;"','") &amp; RC[-2]) &amp;"','") &amp; RC[-1]) &amp; "')"</f>
-        <v>INSERT INTO [Vol].[tblSkill] (SkillID,SkillName,MstrSkillID,ReqCert,ActiveFlg) VALUES('C87F23E9-8F8C-406D-9FBF-E15043179F09','Redditor','6497B3D4-A86F-441C-9856-5E00EB410B9D','1','1')</v>
+        <v>INSERT INTO [Vol].[tblSkill] (SkillID,SkillName,MstrSkillID,ReqCert,ActiveFlg) VALUES('C87F23E9-8F8C-406D-9FBF-E15043179F09','Redditor','153B9006-1488-4CA1-950A-32E28F7B699D','1','1')</v>
       </c>
     </row>
     <row r="4">
@@ -198,13 +186,13 @@
         <v>7</v>
       </c>
       <c t="s" r="B4">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c t="s" r="C4">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c t="s" r="D4">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="E4">
         <v>1</v>
@@ -214,7 +202,7 @@
       </c>
       <c t="str" r="G4">
         <f>((((((((((((((((((((("INSERT INTO " &amp; A4) &amp;" (") &amp; $B$1) &amp; ",") &amp; $C$1) &amp; ",") &amp; $D$1) &amp; ",") &amp; $E$1) &amp; ",") &amp; $F$1) &amp; ") VALUES('") &amp; RC[-5]) &amp;"','") &amp; RC[-4]) &amp;"','") &amp; RC[-3]) &amp;"','") &amp; RC[-2]) &amp;"','") &amp; RC[-1]) &amp; "')"</f>
-        <v>INSERT INTO [Vol].[tblSkill] (SkillID,SkillName,MstrSkillID,ReqCert,ActiveFlg) VALUES('990B091D-6A0D-4543-B766-C37B684F8081','4Chan Troll','F8389EDE-E282-4AAE-B6B7-94A99FF1D85A','1','0')</v>
+        <v>INSERT INTO [Vol].[tblSkill] (SkillID,SkillName,MstrSkillID,ReqCert,ActiveFlg) VALUES('990B091D-6A0D-4543-B766-C37B684F8081','4Chan Troll','C87F23E9-8F8C-406D-9FBF-E15043179F09','1','0')</v>
       </c>
     </row>
   </sheetData>

</xml_diff>